<commit_message>
This logic is for excel
</commit_message>
<xml_diff>
--- a/defect_and_story_count_multiple_projects_2025_02.xlsx
+++ b/defect_and_story_count_multiple_projects_2025_02.xlsx
@@ -1,73 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\ZBB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Defect Count</t>
-  </si>
-  <si>
-    <t>Story Count</t>
-  </si>
-  <si>
-    <t>SCRUM</t>
-  </si>
-  <si>
-    <t>VP</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin"/>
       <right style="thin"/>
@@ -79,16 +56,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -97,10 +141,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -230,7 +274,6 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -254,11 +297,10 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -267,13 +309,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -349,7 +391,6 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -369,76 +410,92 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="12.57031" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28516" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Defect Count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Story Count</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SCRUM</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>2025</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>VP</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>2025</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>